<commit_message>
Popravljao fajlove za PretragaTopPjesama
</commit_message>
<xml_diff>
--- a/UseCaseIScenarij/PretragaTopPjesama.xlsx
+++ b/UseCaseIScenarij/PretragaTopPjesama.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>Naziv</t>
   </si>
@@ -49,15 +49,6 @@
   </si>
   <si>
     <t>Korisnik zatraži da mu se prikažu najslušanije pjesme te sistem formira listu pjesama sa najvećim brojem slušanja u prethodnom mjesecu i prikaže ih korisniku nakon čega on može odabrati neku pjesmu da doda u neki od svojih playlista</t>
-  </si>
-  <si>
-    <t>Korisnik mora imati pristup aplikaciji / web servisu                                                 U bazi podataka mora postojati dovoljan broj pjesama</t>
-  </si>
-  <si>
-    <t>Korisniku je prikazana lista od 10 najslušanijih pjesama posljednji mjesec</t>
-  </si>
-  <si>
-    <t>Korisniku se javlja greška kako nema dovoljno podataka u bazi podataka</t>
   </si>
   <si>
     <t>Korisnik, Sistem</t>
@@ -115,6 +106,9 @@
   </si>
   <si>
     <t>Tok događaja - alternativni tok kada korisnik odabire pjesmu da doda u playlist</t>
+  </si>
+  <si>
+    <t>Korisniku je prikazana lista od 10 najslušanijih pjesama u posljednjem mjesecu</t>
   </si>
 </sst>
 </file>
@@ -503,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -515,7 +509,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -539,15 +533,15 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="57.6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="43.2">
@@ -555,15 +549,15 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="28.8">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -571,7 +565,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -579,15 +573,15 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="57.6">
       <c r="A10" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="57.6">
@@ -595,75 +589,75 @@
         <v>8</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="18">
       <c r="A14" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="28.8">
       <c r="A16" s="8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B16" s="9"/>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="9"/>
       <c r="B17" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="28.8">
       <c r="A18" s="9"/>
       <c r="B18" s="8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="54">
       <c r="A21" s="10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B23" s="9"/>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="9"/>
       <c r="B24" s="9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B25" s="9"/>
     </row>
     <row r="26" spans="1:2" ht="28.8">
       <c r="A26" s="9"/>
       <c r="B26" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>